<commit_message>
matosinhos sem "baseline" (#126)
matosinhos sem "baseline" na descriçao dos cenários. coluna scenario,
tab metrics_metadata
</commit_message>
<xml_diff>
--- a/data/Matosinhos.xlsx
+++ b/data/Matosinhos.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ricardo\Dropbox\BIC Beatriz Godinho\Shapefiles cidades\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB5AC98A-4E4F-46AB-814D-0B4FB847565C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5774335-C947-440E-AB10-A83111B1542D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="metrics" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="817" uniqueCount="727">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="801" uniqueCount="727">
   <si>
     <t>Building_Name</t>
   </si>
@@ -15420,9 +15420,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I17"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I18" sqref="I18"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="18.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.08984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.81640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.81640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
@@ -15475,9 +15488,6 @@
       <c r="H2" t="s">
         <v>704</v>
       </c>
-      <c r="I2" t="s">
-        <v>708</v>
-      </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
@@ -15504,9 +15514,6 @@
       <c r="H3" t="s">
         <v>704</v>
       </c>
-      <c r="I3" t="s">
-        <v>708</v>
-      </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
@@ -15533,9 +15540,6 @@
       <c r="H4" t="s">
         <v>704</v>
       </c>
-      <c r="I4" t="s">
-        <v>708</v>
-      </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
@@ -15562,9 +15566,6 @@
       <c r="H5" t="s">
         <v>704</v>
       </c>
-      <c r="I5" t="s">
-        <v>708</v>
-      </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
@@ -15591,9 +15592,6 @@
       <c r="H6" t="s">
         <v>704</v>
       </c>
-      <c r="I6" t="s">
-        <v>708</v>
-      </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
@@ -15620,9 +15618,6 @@
       <c r="H7" t="s">
         <v>704</v>
       </c>
-      <c r="I7" t="s">
-        <v>708</v>
-      </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
@@ -15649,9 +15644,6 @@
       <c r="H8" t="s">
         <v>704</v>
       </c>
-      <c r="I8" t="s">
-        <v>708</v>
-      </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
@@ -15675,9 +15667,6 @@
       <c r="H9" t="s">
         <v>705</v>
       </c>
-      <c r="I9" t="s">
-        <v>708</v>
-      </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
@@ -15704,9 +15693,6 @@
       <c r="H10" t="s">
         <v>705</v>
       </c>
-      <c r="I10" t="s">
-        <v>708</v>
-      </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
@@ -15733,9 +15719,6 @@
       <c r="H11" t="s">
         <v>705</v>
       </c>
-      <c r="I11" t="s">
-        <v>708</v>
-      </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
@@ -15759,9 +15742,6 @@
       <c r="H12" t="s">
         <v>706</v>
       </c>
-      <c r="I12" t="s">
-        <v>708</v>
-      </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
@@ -15788,9 +15768,6 @@
       <c r="H13" t="s">
         <v>706</v>
       </c>
-      <c r="I13" t="s">
-        <v>708</v>
-      </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
@@ -15817,9 +15794,6 @@
       <c r="H14" t="s">
         <v>706</v>
       </c>
-      <c r="I14" t="s">
-        <v>708</v>
-      </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
@@ -15843,9 +15817,6 @@
       <c r="H15" t="s">
         <v>707</v>
       </c>
-      <c r="I15" t="s">
-        <v>708</v>
-      </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
@@ -15872,11 +15843,8 @@
       <c r="H16" t="s">
         <v>707</v>
       </c>
-      <c r="I16" t="s">
-        <v>708</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>668</v>
       </c>
@@ -15900,9 +15868,6 @@
       </c>
       <c r="H17" t="s">
         <v>707</v>
-      </c>
-      <c r="I17" t="s">
-        <v>708</v>
       </c>
     </row>
   </sheetData>
@@ -15914,11 +15879,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="14.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="58.6328125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">

</xml_diff>